<commit_message>
Grouping of vars according to scripts.
</commit_message>
<xml_diff>
--- a/excel-in/calculations.xlsx
+++ b/excel-in/calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\adb.intra.admin.ch\Userhome$\AGROSCOPE-01\U80823148\config\Desktop\aktuell\mimi_Excel-Export\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B621575-3BB8-4DEF-9718-96C23B8EBC72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A522DFC2-6930-4920-91A3-0745D26FA962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3705" yWindow="2295" windowWidth="20550" windowHeight="13185" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3705" yWindow="2295" windowWidth="20550" windowHeight="13185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="calculations1" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <definedName name="f">calculations2!$C$3</definedName>
     <definedName name="g">calculations2!$C$4</definedName>
     <definedName name="h">calculations2!$C$5</definedName>
+    <definedName name="x">calculations1!$C$6</definedName>
     <definedName name="z_">calculations2!$C$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -92,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>a</t>
   </si>
@@ -119,6 +120,9 @@
   </si>
   <si>
     <t>h</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -443,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:C5"/>
+  <dimension ref="B2:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,6 +489,15 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <f>z_+1</f>
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Titel Eingabemeldung" prompt="Text Eingabemeldung" sqref="C3" xr:uid="{E1E8322D-9FF5-4D02-BF25-75E019D4D4AD}"/>
@@ -498,7 +511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43E6F323-4317-455B-9326-3F1D17DE4FC0}">
   <dimension ref="B2:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Improved grouping according to sheets. Added possibility to include comments as well as left and right cell values into final script (as comments).
</commit_message>
<xml_diff>
--- a/excel-in/calculations.xlsx
+++ b/excel-in/calculations.xlsx
@@ -5,16 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\adb.intra.admin.ch\Userhome$\AGROSCOPE-01\U80823148\config\Desktop\aktuell\mimi_Excel-Export\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U80823148\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A522DFC2-6930-4920-91A3-0745D26FA962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8494879D-A7BB-4015-8307-D92CEA507B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3705" yWindow="2295" windowWidth="20550" windowHeight="13185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1290" yWindow="-120" windowWidth="27630" windowHeight="18240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="calculations1" sheetId="1" r:id="rId1"/>
-    <sheet name="calculations2" sheetId="2" r:id="rId2"/>
+    <sheet name="calculations2" sheetId="2" r:id="rId1"/>
+    <sheet name="a" sheetId="3" r:id="rId2"/>
+    <sheet name="b" sheetId="4" r:id="rId3"/>
+    <sheet name="calculations1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="a">calculations1!$C$2</definedName>
@@ -25,7 +27,9 @@
     <definedName name="f">calculations2!$C$3</definedName>
     <definedName name="g">calculations2!$C$4</definedName>
     <definedName name="h">calculations2!$C$5</definedName>
+    <definedName name="w">b!$C$5</definedName>
     <definedName name="x">calculations1!$C$6</definedName>
+    <definedName name="y">a!$C$5</definedName>
     <definedName name="z_">calculations2!$C$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -52,17 +56,98 @@
     <author>Hoop Daniel Agroscope</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{23F92A9E-2BE5-44E4-B777-AECF82E7D77E}">
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{74C51C12-EE91-4FA5-8551-81B4C31ED991}">
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
             <charset val="1"/>
           </rPr>
-          <t>Kommentar a</t>
+          <t>calculations2.z_</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Hoop Daniel Agroscope</author>
+  </authors>
+  <commentList>
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{F2FBE97B-6D73-479B-B562-8BA56C2CD9FE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>a.y</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Hoop Daniel Agroscope</author>
+  </authors>
+  <commentList>
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{B592EBD7-9E61-446F-83CA-69A308206197}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>b.w</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Hoop Daniel Agroscope</author>
+  </authors>
+  <commentList>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{23F92A9E-2BE5-44E4-B777-AECF82E7D77E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>calculations1.a</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{218F22E9-7DE0-4564-B72D-7980C032D98F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>calculations1.x</t>
         </r>
       </text>
     </comment>
@@ -93,7 +178,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>a</t>
   </si>
@@ -123,13 +208,22 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Finaler Wert</t>
+  </si>
+  <si>
+    <t>w</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,11 +232,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Segoe UI"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -446,11 +545,123 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43E6F323-4317-455B-9326-3F1D17DE4FC0}">
+  <dimension ref="B2:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <f>e+f+a</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <f>e+f+a</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" cm="1">
+        <f t="array" ref="C6">h+1</f>
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E0E01F-80DD-47AF-A38E-49101BB19862}">
+  <dimension ref="B5:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <f>x+z_+w</f>
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E8C5A8A-CC39-4F9C-881C-EC85C00F4341}">
+  <dimension ref="B5:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,64 +714,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Titel Eingabemeldung" prompt="Text Eingabemeldung" sqref="C3" xr:uid="{E1E8322D-9FF5-4D02-BF25-75E019D4D4AD}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43E6F323-4317-455B-9326-3F1D17DE4FC0}">
-  <dimension ref="B2:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <f>e+f+a</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <f>e+f+a</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" cm="1">
-        <f t="array" ref="C6">h+1</f>
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Can also read variables of which the names were not defined.
</commit_message>
<xml_diff>
--- a/excel-in/calculations.xlsx
+++ b/excel-in/calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U80823148\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8494879D-A7BB-4015-8307-D92CEA507B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9F9FB9-2896-42C1-AF75-70B592ABBCC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1290" yWindow="-120" windowWidth="27630" windowHeight="18240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,6 +27,8 @@
     <definedName name="f">calculations2!$C$3</definedName>
     <definedName name="g">calculations2!$C$4</definedName>
     <definedName name="h">calculations2!$C$5</definedName>
+    <definedName name="i">calculations1!$C$10</definedName>
+    <definedName name="j">calculations1!$C$11</definedName>
     <definedName name="w">b!$C$5</definedName>
     <definedName name="x">calculations1!$C$6</definedName>
     <definedName name="y">a!$C$5</definedName>
@@ -658,10 +660,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:C6"/>
+  <dimension ref="B2:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,6 +708,52 @@
       </c>
       <c r="C6">
         <f>z_+1</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <f>C8+1</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <f>C8+1</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <f>C9+1</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <f>C10+1</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <f>i+1</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <f>C8+1</f>
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Now also works with HLOOKUP, VLOOKUP / WVERWEIS, SVERWEIS
</commit_message>
<xml_diff>
--- a/excel-in/calculations.xlsx
+++ b/excel-in/calculations.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U80823148\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Data-Work\25_Agricultural_Economics-RE\251_ZA-BH_protected\AblagePers\hpda\tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9F9FB9-2896-42C1-AF75-70B592ABBCC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1290" yWindow="-120" windowWidth="27630" windowHeight="18240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1410" yWindow="0" windowWidth="27390" windowHeight="12885" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="calculations2" sheetId="2" r:id="rId1"/>
@@ -34,7 +33,7 @@
     <definedName name="y">a!$C$5</definedName>
     <definedName name="z_">calculations2!$C$6</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -53,12 +52,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Hoop Daniel Agroscope</author>
   </authors>
   <commentList>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{74C51C12-EE91-4FA5-8551-81B4C31ED991}">
+    <comment ref="C6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -76,12 +75,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Hoop Daniel Agroscope</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{F2FBE97B-6D73-479B-B562-8BA56C2CD9FE}">
+    <comment ref="C5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -99,12 +98,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Hoop Daniel Agroscope</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{B592EBD7-9E61-446F-83CA-69A308206197}">
+    <comment ref="C5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -122,12 +121,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Hoop Daniel Agroscope</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{23F92A9E-2BE5-44E4-B777-AECF82E7D77E}">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -140,7 +139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{218F22E9-7DE0-4564-B72D-7980C032D98F}">
+    <comment ref="C6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -158,14 +157,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -180,7 +179,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>a</t>
   </si>
@@ -220,11 +219,26 @@
   <si>
     <t>w</t>
   </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>SVERWEIS</t>
+  </si>
+  <si>
+    <t>WVERWEIS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -547,7 +561,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43E6F323-4317-455B-9326-3F1D17DE4FC0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -606,7 +620,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E0E01F-80DD-47AF-A38E-49101BB19862}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -635,7 +649,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E8C5A8A-CC39-4F9C-881C-EC85C00F4341}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -659,16 +673,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:C16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -677,7 +691,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -685,7 +699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -694,7 +708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -702,7 +716,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -710,56 +724,142 @@
         <f>z_+1</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>3</v>
+      </c>
+      <c r="K8">
+        <v>4</v>
+      </c>
+      <c r="L8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C9">
         <f>C8+1</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9">
+        <v>6</v>
+      </c>
+      <c r="K9">
+        <v>7</v>
+      </c>
+      <c r="L9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C10">
         <f>C8+1</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>9</v>
+      </c>
+      <c r="K10">
+        <v>10</v>
+      </c>
+      <c r="L10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C13">
         <f>C9+1</f>
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C14">
         <f>C10+1</f>
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C15">
         <f>i+1</f>
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C16">
         <f>C8+1</f>
         <v>11</v>
       </c>
     </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <f>VLOOKUP("a",$I$6:$L$10,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <f>HLOOKUP(3,$I$6:$L$10,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Titel Eingabemeldung" prompt="Text Eingabemeldung" sqref="C3" xr:uid="{E1E8322D-9FF5-4D02-BF25-75E019D4D4AD}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Titel Eingabemeldung" prompt="Text Eingabemeldung" sqref="C3"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Significant improvements in handling (H|V)LOOKUP / (S|W)VERWEIS. Also writing logs.
</commit_message>
<xml_diff>
--- a/excel-in/calculations.xlsx
+++ b/excel-in/calculations.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="0" windowWidth="27390" windowHeight="12885" activeTab="3"/>
+    <workbookView xWindow="2820" yWindow="0" windowWidth="27390" windowHeight="12885" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="calculations2" sheetId="2" r:id="rId1"/>
     <sheet name="a" sheetId="3" r:id="rId2"/>
     <sheet name="b" sheetId="4" r:id="rId3"/>
     <sheet name="calculations1" sheetId="1" r:id="rId4"/>
+    <sheet name="lookup_a" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="a">calculations1!$C$2</definedName>
@@ -28,6 +29,7 @@
     <definedName name="h">calculations2!$C$5</definedName>
     <definedName name="i">calculations1!$C$10</definedName>
     <definedName name="j">calculations1!$C$11</definedName>
+    <definedName name="r_">calculations1!$C$21</definedName>
     <definedName name="w">b!$C$5</definedName>
     <definedName name="x">calculations1!$C$6</definedName>
     <definedName name="y">a!$C$5</definedName>
@@ -156,6 +158,40 @@
 </comments>
 </file>
 
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Hoop Daniel</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Hoop Daniel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
@@ -179,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>a</t>
   </si>
@@ -214,9 +250,6 @@
     <t>y</t>
   </si>
   <si>
-    <t>Finaler Wert</t>
-  </si>
-  <si>
     <t>w</t>
   </si>
   <si>
@@ -229,17 +262,83 @@
     <t>t</t>
   </si>
   <si>
-    <t>SVERWEIS</t>
-  </si>
-  <si>
-    <t>WVERWEIS</t>
+    <t>s</t>
+  </si>
+  <si>
+    <t>is defined as i</t>
+  </si>
+  <si>
+    <t>is defined as e</t>
+  </si>
+  <si>
+    <t>is defined as f</t>
+  </si>
+  <si>
+    <t>is defined as g</t>
+  </si>
+  <si>
+    <t>is defined as h</t>
+  </si>
+  <si>
+    <t>is defined as z_</t>
+  </si>
+  <si>
+    <t>is defined as w</t>
+  </si>
+  <si>
+    <t>final value</t>
+  </si>
+  <si>
+    <t>is defined as a</t>
+  </si>
+  <si>
+    <t>is defined as b</t>
+  </si>
+  <si>
+    <t>is defined as c_</t>
+  </si>
+  <si>
+    <t>is defined as d</t>
+  </si>
+  <si>
+    <t>is defined as x</t>
+  </si>
+  <si>
+    <t>is defined as j</t>
+  </si>
+  <si>
+    <t>VLOOKUP / SVERWEIS</t>
+  </si>
+  <si>
+    <t>HLOOKUP / WVERWEIS</t>
+  </si>
+  <si>
+    <t>VLOOKUP / SVERWEIS - using variable</t>
+  </si>
+  <si>
+    <t>r_</t>
+  </si>
+  <si>
+    <t>variable for VLOOKUP</t>
+  </si>
+  <si>
+    <t>u2</t>
+  </si>
+  <si>
+    <t>VLOOKUP / SVERWEIS (duplicate)</t>
+  </si>
+  <si>
+    <t>This sheet will be discarded because of the sheet name.</t>
+  </si>
+  <si>
+    <t>should become VAR_</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,6 +357,13 @@
       <color indexed="81"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -280,8 +386,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -562,31 +671,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C6"/>
+  <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -594,8 +709,11 @@
         <f>e+f+a</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -603,14 +721,20 @@
         <f>e+f+a</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" cm="1">
         <f t="array" ref="C6">h+1</f>
         <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -624,7 +748,7 @@
   <dimension ref="B5:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,7 +762,7 @@
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -650,20 +774,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:C5"/>
+  <dimension ref="B5:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -674,11 +801,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L18"/>
+  <dimension ref="B2:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -690,6 +815,9 @@
         <f>IF(b&lt;10,b+c_,0)</f>
         <v>6</v>
       </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -698,6 +826,9 @@
       <c r="C3">
         <v>1</v>
       </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -707,6 +838,9 @@
         <f>d+1</f>
         <v>5</v>
       </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -715,6 +849,9 @@
       <c r="C5">
         <v>4</v>
       </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -724,6 +861,9 @@
         <f>z_+1</f>
         <v>11</v>
       </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
       <c r="I6">
         <v>1</v>
       </c>
@@ -754,6 +894,9 @@
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
       </c>
       <c r="I8" t="s">
         <v>1</v>
@@ -773,8 +916,11 @@
         <f>C8+1</f>
         <v>11</v>
       </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
       <c r="I9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J9">
         <v>6</v>
@@ -791,6 +937,9 @@
         <f>C8+1</f>
         <v>11</v>
       </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
       <c r="I10" t="s">
         <v>2</v>
       </c>
@@ -807,6 +956,9 @@
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
@@ -814,47 +966,140 @@
         <f>C9+1</f>
         <v>12</v>
       </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C14">
         <f>C10+1</f>
         <v>12</v>
       </c>
+      <c r="D14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C15">
         <f>i+1</f>
         <v>12</v>
       </c>
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15">
+        <v>3</v>
+      </c>
+      <c r="K15">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C16">
         <f>C8+1</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16" t="s">
+        <v>5</v>
+      </c>
+      <c r="J16">
+        <v>6</v>
+      </c>
+      <c r="K16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17">
         <f>VLOOKUP("a",$I$6:$L$10,2,FALSE)</f>
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="I17" t="s">
+        <v>8</v>
+      </c>
+      <c r="J17">
+        <v>9</v>
+      </c>
+      <c r="K17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C18">
+        <f>VLOOKUP("a",$I$6:$L$10,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19">
         <f>HLOOKUP(3,$I$6:$L$10,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="D18" t="s">
-        <v>17</v>
+      <c r="D19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20">
+        <f>VLOOKUP(r_,$I$13:$L$17,2,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="1" t="str">
+        <f>"h"</f>
+        <v>h</v>
+      </c>
+      <c r="D21" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -865,4 +1110,25 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>